<commit_message>
Auto commit - 10281111
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$89</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="616">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-23  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="679">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-28  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1910,6 +1910,202 @@
   </si>
   <si>
     <t>2025-10-23 11:30:00</t>
+  </si>
+  <si>
+    <t>E4680114102301</t>
+  </si>
+  <si>
+    <t>2025-10-23 19:27:16</t>
+  </si>
+  <si>
+    <t>HLM3</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET 標籤印表機</t>
+  </si>
+  <si>
+    <t>M301</t>
+  </si>
+  <si>
+    <t>門市反應MMK標籤印表機亮紅燈且不會自動裁紙,已有請門市將票券機線路重新拔插紙捲重放仍無法排除.......還請台芝到店協助(印ec的機器故障)</t>
+  </si>
+  <si>
+    <t>2025-10-23 19:40:26</t>
+  </si>
+  <si>
+    <t>2025-10-27 16:56:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 17:29:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 23:40:00</t>
+  </si>
+  <si>
+    <t>更換標籤機
+換上：8187001030
+換下：8187000916</t>
+  </si>
+  <si>
+    <t>E4552114102501</t>
+  </si>
+  <si>
+    <t>新莊福慧店</t>
+  </si>
+  <si>
+    <t>2025-10-25 10:54:24</t>
+  </si>
+  <si>
+    <t>HL25</t>
+  </si>
+  <si>
+    <t>HL-SC螢幕</t>
+  </si>
+  <si>
+    <t>螢幕畫面閃爍頻繁或無畫面</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應SC螢幕(LCD)右半邊有黑一塊，切到監視器畫面也是，已有重啟SC、重新拔插螢幕線路仍異常...請台芝到店協助(螢幕有部分黑黑的)
+</t>
+  </si>
+  <si>
+    <t>THILF04552</t>
+  </si>
+  <si>
+    <t>2025-10-25 11:06:27</t>
+  </si>
+  <si>
+    <t>2025-10-27 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 13:00:00</t>
+  </si>
+  <si>
+    <t>更換螢幕
+換上8133003736
+換下8133002651</t>
+  </si>
+  <si>
+    <t>E3957114102501</t>
+  </si>
+  <si>
+    <t>三重福仁店</t>
+  </si>
+  <si>
+    <t>2025-10-25 13:05:00</t>
+  </si>
+  <si>
+    <t>抽屜無法正常開關</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm1收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中)、鎖頭編號:5001)抽屜關不起來，會自動彈開..請台芝到店協助(機台1收銀機無法關起來)
+</t>
+  </si>
+  <si>
+    <t>THILF03957</t>
+  </si>
+  <si>
+    <t>2025-10-25 13:16:52</t>
+  </si>
+  <si>
+    <t>2025-10-27 10:08:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 10:38:00</t>
+  </si>
+  <si>
+    <t>14406114102501</t>
+  </si>
+  <si>
+    <t>板橋稚暉店</t>
+  </si>
+  <si>
+    <t>2025-10-25 16:50:38</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)突然黑屏，無法開機且螢幕右下方沒有亮燈，門市告知因現場線路繁亂無法確認電源線是哪一條，ping81不通無法vnc...需請台芝到店協助 
+與門市確認10/25已清帳，清帳後有交易PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>THILF04406</t>
+  </si>
+  <si>
+    <t>2025-10-25 16:59:21</t>
+  </si>
+  <si>
+    <t>2025-10-27 17:02:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 17:32:00</t>
+  </si>
+  <si>
+    <t>14144114102701</t>
+  </si>
+  <si>
+    <t>新莊頭前店</t>
+  </si>
+  <si>
+    <t>2025-10-27 09:12:59</t>
+  </si>
+  <si>
+    <t>滑鼠故障無作用</t>
+  </si>
+  <si>
+    <t>門市反應SC滑鼠感應不良常常點了無反應，門市找不到後方線路無法重新拔插...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04144</t>
+  </si>
+  <si>
+    <t>2025-10-27 09:15:09</t>
+  </si>
+  <si>
+    <t>2025-10-27 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 16:10:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 13:15:00</t>
+  </si>
+  <si>
+    <t>更換滑鼠</t>
+  </si>
+  <si>
+    <t>13840114102701</t>
+  </si>
+  <si>
+    <t>2025-10-27 09:53:56</t>
+  </si>
+  <si>
+    <t>mmk4代機-門市反應消費者操作MMK生活服務&gt;店到店寄件&gt;HILIFE店到店&gt;立即寄件無代碼&gt;消費者輸入資料後選擇寄件門市4652 三重商工店&gt;列印寄件單後畫面當掉無反應也未列印寄件單，已協助遠端重啟後再次操作仍異常，經總公司功評確認:請先行派工到店更換MMK硬碟後，請門市當下操作測試確認是否有問題，若仍異常請台芝廠商現場協助錄影提供總公司確認...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-10-27 09:57:02</t>
+  </si>
+  <si>
+    <t>2025-10-27 15:08:00</t>
+  </si>
+  <si>
+    <t>2025-10-27 15:38:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 13:57:00</t>
+  </si>
+  <si>
+    <t>現場已經更換MMK硬碟，依然出現無法列印的狀況，已經錄影傳至維修群組</t>
+  </si>
+  <si>
+    <t>2025-10-27 17:16:31</t>
+  </si>
+  <si>
+    <t>2025-10-27 17:17:45</t>
+  </si>
+  <si>
+    <t>2025-10-27 16:30:00</t>
   </si>
 </sst>
 </file>
@@ -2323,10 +2519,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK89"/>
+  <dimension ref="A1:AK97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A89" sqref="A89"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9832,7 +10028,7 @@
       <c r="M89" s="8"/>
       <c r="N89" s="7"/>
       <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
+      <c r="P89" s="9"/>
       <c r="Q89" s="7" t="s">
         <v>586</v>
       </c>
@@ -9865,7 +10061,7 @@
       <c r="AB89" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC89" s="8" t="s">
+      <c r="AC89" s="9" t="s">
         <v>95</v>
       </c>
       <c r="AD89" s="7" t="s">
@@ -9878,6 +10074,742 @@
       <c r="AI89" s="7"/>
       <c r="AJ89" s="7"/>
       <c r="AK89" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2025103112</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="3">
+        <v>4680</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2025103121</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="7">
+        <v>4552</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L91" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="M91" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="N91" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O91" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="Q91" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="Y91" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z91" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2025103122</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F92" s="3">
+        <v>3957</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N92" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O92" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="P92" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="Y92" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z92" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="AD92" s="3"/>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2025103124</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F93" s="7">
+        <v>4406</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="K93" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L93" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M93" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N93" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O93" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P93" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="Q93" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="Y93" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="Z93" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC93" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD93" s="7"/>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2025103131</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="3">
+        <v>4144</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="N94" s="3">
+        <v>2403</v>
+      </c>
+      <c r="O94" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="R94" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T94" s="3">
+        <v>1</v>
+      </c>
+      <c r="U94" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V94" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="X94" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="Y94" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="Z94" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="AD94" s="3"/>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+      <c r="AJ94" s="3"/>
+      <c r="AK94" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" s="7">
+        <v>2025103156</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="7">
+        <v>3840</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="K95" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L95" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="M95" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="N95" s="7">
+        <v>5803</v>
+      </c>
+      <c r="O95" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="P95" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q95" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="R95" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T95" s="7">
+        <v>1</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V95" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="W95" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="X95" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="Y95" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="Z95" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC95" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="AD95" s="7"/>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="7"/>
+      <c r="AG95" s="7"/>
+      <c r="AH95" s="7"/>
+      <c r="AI95" s="7"/>
+      <c r="AJ95" s="7"/>
+      <c r="AK95" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2025103275</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <v>4552</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S96" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T96" s="3">
+        <v>1</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V96" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="X96" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD96" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+      <c r="AJ96" s="3"/>
+      <c r="AK96" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2025103278</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7">
+        <v>4144</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC97" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD97" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7"/>
+      <c r="AK97" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10281238
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$102</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="705">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-28  )</t>
   </si>
@@ -2106,6 +2106,84 @@
   </si>
   <si>
     <t>2025-10-27 16:30:00</t>
+  </si>
+  <si>
+    <t>D649</t>
+  </si>
+  <si>
+    <t>三重運動公園</t>
+  </si>
+  <si>
+    <t>THILF0D649</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:13:24</t>
+  </si>
+  <si>
+    <t>2025-10-28 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 10:50:00</t>
+  </si>
+  <si>
+    <t>PMQ4+L90</t>
+  </si>
+  <si>
+    <t>北縣泰富店</t>
+  </si>
+  <si>
+    <t>新北市泰山區</t>
+  </si>
+  <si>
+    <t>THILF03606</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:14:45</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:00:00</t>
+  </si>
+  <si>
+    <t>泰山新民店</t>
+  </si>
+  <si>
+    <t>THILF04656</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:33:15</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:54:28</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:05:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 11:20:00</t>
+  </si>
+  <si>
+    <t>L90</t>
+  </si>
+  <si>
+    <t>D028</t>
+  </si>
+  <si>
+    <t>三重正義北店</t>
+  </si>
+  <si>
+    <t>THILF0D028</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:32:58</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:20:00</t>
   </si>
 </sst>
 </file>
@@ -2519,10 +2597,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK97"/>
+  <dimension ref="A1:AK102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="AC99" sqref="AC99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10764,7 +10842,7 @@
       <c r="M97" s="8"/>
       <c r="N97" s="7"/>
       <c r="O97" s="8"/>
-      <c r="P97" s="8"/>
+      <c r="P97" s="9"/>
       <c r="Q97" s="7" t="s">
         <v>662</v>
       </c>
@@ -10797,7 +10875,7 @@
       <c r="AB97" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC97" s="8" t="s">
+      <c r="AC97" s="9" t="s">
         <v>95</v>
       </c>
       <c r="AD97" s="7" t="s">
@@ -10810,6 +10888,393 @@
       <c r="AI97" s="7"/>
       <c r="AJ97" s="7"/>
       <c r="AK97" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2025103336</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="Y98" s="3"/>
+      <c r="Z98" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC98" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3"/>
+      <c r="AK98" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2025103337</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7">
+        <v>3606</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="Y99" s="7"/>
+      <c r="Z99" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC99" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD99" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7"/>
+      <c r="AK99" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2025103342</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3">
+        <v>4656</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK100" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2025103348</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7">
+        <v>5377</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="9"/>
+      <c r="Q101" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y101" s="7"/>
+      <c r="Z101" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="AD101" s="7"/>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK101" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2025103349</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC102" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD102" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3"/>
+      <c r="AK102" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10281847
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$102</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$114</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="767">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-28  )</t>
   </si>
@@ -2108,6 +2108,42 @@
     <t>2025-10-27 16:30:00</t>
   </si>
   <si>
+    <t>1D349114102701</t>
+  </si>
+  <si>
+    <t>D349</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
+    <t>2025-10-27 19:26:49</t>
+  </si>
+  <si>
+    <t>客顯示器畫面不正常</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)客顯螢幕黑頻,確認右下角燈號為藍燈,已有重新開關機仍無法排除,點選電源鍵關閉重開亦無法排除............還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>2025-10-27 19:28:18</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:45:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 23:28:00</t>
+  </si>
+  <si>
+    <t>驅動修復測試正常，請門市觀察中</t>
+  </si>
+  <si>
     <t>D649</t>
   </si>
   <si>
@@ -2184,6 +2220,157 @@
   </si>
   <si>
     <t>2025-10-28 12:20:00</t>
+  </si>
+  <si>
+    <t>三重大院店</t>
+  </si>
+  <si>
+    <t>THILF04560</t>
+  </si>
+  <si>
+    <t>2025-10-28 13:14:52</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:50:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 13:14:00</t>
+  </si>
+  <si>
+    <t>三重夜市口</t>
+  </si>
+  <si>
+    <t>THILF02935</t>
+  </si>
+  <si>
+    <t>2025-10-28 14:29:28</t>
+  </si>
+  <si>
+    <t>2025-10-28 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 14:28:00</t>
+  </si>
+  <si>
+    <t>林口捷韻店</t>
+  </si>
+  <si>
+    <t>新北市林口區</t>
+  </si>
+  <si>
+    <t>THILF04715</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:08:35</t>
+  </si>
+  <si>
+    <t>2025-10-28 14:30:00</t>
+  </si>
+  <si>
+    <t>三重中央北店</t>
+  </si>
+  <si>
+    <t>THILF02042</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:18:26</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:17:00</t>
+  </si>
+  <si>
+    <t>14154114102802</t>
+  </si>
+  <si>
+    <t>林口麗園店</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:32:06</t>
+  </si>
+  <si>
+    <t>2025/10/28 (週二) 下午 03:28 總公司明翰 mail:mmk4代機有關4154林口麗園店- LIFEET列印藥師少女的獨語未印出 (案14154114102801)經查結果，門市LIFE-ET硬碟故障，請協助一般派工，更換MMK硬碟並重新安裝，謝謝。</t>
+  </si>
+  <si>
+    <t>THILF04154</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:33:52</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 16:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 19:33:00</t>
+  </si>
+  <si>
+    <t>更換硬碟 
+以再生龍重裝系統</t>
+  </si>
+  <si>
+    <t>15364114102801</t>
+  </si>
+  <si>
+    <t>林口舊街店</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:25:04</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)突然無畫面，右下角無亮燈，門市已嘗試重新拔插電源線及變壓器線路仍異常，PING80不通，與門市確認粉色插座以手機充電測試有通電...需請台芝到店協助，與門市確認入帳日10/29有交易資料，PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確</t>
+  </si>
+  <si>
+    <t>THILF05364</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:37:08</t>
+  </si>
+  <si>
+    <t>2025-10-28 17:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 18:40:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 19:37:00</t>
+  </si>
+  <si>
+    <t>供電異常導致主機開機error&amp;螢幕顯示異常，經放電後測試功能正常，請門市觀察中</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:48:53</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:46:00</t>
+  </si>
+  <si>
+    <t>三重三和夜市</t>
+  </si>
+  <si>
+    <t>THILF02303</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:50:02</t>
+  </si>
+  <si>
+    <t>2025-10-28 14:20:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:51:32</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 16:38:44</t>
+  </si>
+  <si>
+    <t>2025-10-28 17:32:50</t>
+  </si>
+  <si>
+    <t>PMQ4+L99</t>
   </si>
 </sst>
 </file>
@@ -2597,10 +2784,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK102"/>
+  <dimension ref="A1:AK114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC99" sqref="AC99"/>
+      <selection activeCell="AC111" sqref="AC111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10896,38 +11083,58 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C98" s="3">
-        <v>2025103336</v>
-      </c>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
+        <v>2025103297</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F98" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N98" s="3">
+        <v>2302</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>684</v>
+      </c>
       <c r="Q98" s="3" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="R98" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S98" s="3" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="T98" s="3">
         <v>1</v>
@@ -10936,28 +11143,28 @@
         <v>54</v>
       </c>
       <c r="V98" s="3" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="W98" s="3" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="X98" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="Y98" s="3"/>
+        <v>688</v>
+      </c>
+      <c r="Y98" s="3" t="s">
+        <v>689</v>
+      </c>
       <c r="Z98" s="3">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="AA98" s="3"/>
       <c r="AB98" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC98" s="10" t="s">
-        <v>685</v>
-      </c>
-      <c r="AD98" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="AD98" s="3"/>
       <c r="AE98" s="3"/>
       <c r="AF98" s="3"/>
       <c r="AG98" s="3"/>
@@ -10976,18 +11183,18 @@
         <v>92</v>
       </c>
       <c r="C99" s="7">
-        <v>2025103337</v>
+        <v>2025103336</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
-      <c r="F99" s="7">
-        <v>3606</v>
+      <c r="F99" s="7" t="s">
+        <v>691</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>687</v>
+        <v>98</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
@@ -10998,13 +11205,13 @@
       <c r="O99" s="8"/>
       <c r="P99" s="9"/>
       <c r="Q99" s="7" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="R99" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S99" s="7" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="T99" s="7">
         <v>1</v>
@@ -11013,24 +11220,24 @@
         <v>54</v>
       </c>
       <c r="V99" s="7" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="W99" s="7" t="s">
-        <v>683</v>
+        <v>695</v>
       </c>
       <c r="X99" s="7" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="Y99" s="7"/>
       <c r="Z99" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA99" s="7"/>
       <c r="AB99" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC99" s="9" t="s">
-        <v>95</v>
+        <v>697</v>
       </c>
       <c r="AD99" s="7" t="s">
         <v>61</v>
@@ -11053,18 +11260,18 @@
         <v>92</v>
       </c>
       <c r="C100" s="3">
-        <v>2025103342</v>
+        <v>2025103337</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3">
-        <v>4656</v>
+        <v>3606</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>691</v>
+        <v>698</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>687</v>
+        <v>699</v>
       </c>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
@@ -11075,7 +11282,7 @@
       <c r="O100" s="4"/>
       <c r="P100" s="10"/>
       <c r="Q100" s="3" t="s">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="R100" s="3" t="s">
         <v>52</v>
@@ -11090,13 +11297,13 @@
         <v>54</v>
       </c>
       <c r="V100" s="3" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
       <c r="W100" s="3" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
       <c r="X100" s="3" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
       <c r="Y100" s="3"/>
       <c r="Z100" s="3">
@@ -11107,7 +11314,7 @@
         <v>59</v>
       </c>
       <c r="AC100" s="10" t="s">
-        <v>685</v>
+        <v>95</v>
       </c>
       <c r="AD100" s="3" t="s">
         <v>61</v>
@@ -11117,9 +11324,7 @@
       <c r="AG100" s="3"/>
       <c r="AH100" s="3"/>
       <c r="AI100" s="3"/>
-      <c r="AJ100" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ100" s="3"/>
       <c r="AK100" s="3" t="s">
         <v>61</v>
       </c>
@@ -11132,18 +11337,18 @@
         <v>92</v>
       </c>
       <c r="C101" s="7">
-        <v>2025103348</v>
+        <v>2025103342</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7">
-        <v>5377</v>
+        <v>4656</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>503</v>
+        <v>703</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>98</v>
+        <v>699</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
@@ -11154,13 +11359,13 @@
       <c r="O101" s="8"/>
       <c r="P101" s="9"/>
       <c r="Q101" s="7" t="s">
-        <v>504</v>
+        <v>704</v>
       </c>
       <c r="R101" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S101" s="7" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="T101" s="7">
         <v>1</v>
@@ -11169,26 +11374,28 @@
         <v>54</v>
       </c>
       <c r="V101" s="7" t="s">
-        <v>695</v>
+        <v>705</v>
       </c>
       <c r="W101" s="7" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="X101" s="7" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="Y101" s="7"/>
       <c r="Z101" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA101" s="7"/>
       <c r="AB101" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC101" s="9" t="s">
-        <v>698</v>
-      </c>
-      <c r="AD101" s="7"/>
+        <v>697</v>
+      </c>
+      <c r="AD101" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AE101" s="7"/>
       <c r="AF101" s="7"/>
       <c r="AG101" s="7"/>
@@ -11209,15 +11416,15 @@
         <v>92</v>
       </c>
       <c r="C102" s="3">
-        <v>2025103349</v>
+        <v>2025103348</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="3" t="s">
-        <v>699</v>
+      <c r="F102" s="3">
+        <v>5377</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>700</v>
+        <v>503</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>98</v>
@@ -11229,9 +11436,9 @@
       <c r="M102" s="4"/>
       <c r="N102" s="3"/>
       <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
+      <c r="P102" s="10"/>
       <c r="Q102" s="3" t="s">
-        <v>701</v>
+        <v>504</v>
       </c>
       <c r="R102" s="3" t="s">
         <v>52</v>
@@ -11246,13 +11453,13 @@
         <v>54</v>
       </c>
       <c r="V102" s="3" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
       <c r="W102" s="3" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="X102" s="3" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="Y102" s="3"/>
       <c r="Z102" s="3">
@@ -11262,19 +11469,987 @@
       <c r="AB102" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC102" s="4" t="s">
-        <v>685</v>
-      </c>
-      <c r="AD102" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AC102" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="AD102" s="3"/>
       <c r="AE102" s="3"/>
       <c r="AF102" s="3"/>
       <c r="AG102" s="3"/>
       <c r="AH102" s="3"/>
       <c r="AI102" s="3"/>
-      <c r="AJ102" s="3"/>
+      <c r="AJ102" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="AK102" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2025103349</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC103" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD103" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7"/>
+      <c r="AK103" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2025103352</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3">
+        <v>4560</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="10"/>
+      <c r="Q104" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC104" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD104" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3"/>
+      <c r="AK104" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:37">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C105" s="7">
+        <v>2025103356</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7">
+        <v>2935</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="8"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="8"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T105" s="7">
+        <v>1</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V105" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="W105" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="X105" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="Y105" s="7"/>
+      <c r="Z105" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC105" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD105" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="7"/>
+      <c r="AG105" s="7"/>
+      <c r="AH105" s="7"/>
+      <c r="AI105" s="7"/>
+      <c r="AJ105" s="7"/>
+      <c r="AK105" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:37">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2025103369</v>
+      </c>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3">
+        <v>4715</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="10"/>
+      <c r="Q106" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T106" s="3">
+        <v>1</v>
+      </c>
+      <c r="U106" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V106" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="X106" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="Y106" s="3"/>
+      <c r="Z106" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC106" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD106" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK106" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:37">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C107" s="7">
+        <v>2025103375</v>
+      </c>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7">
+        <v>2042</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="8"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="8"/>
+      <c r="P107" s="9"/>
+      <c r="Q107" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T107" s="7">
+        <v>1</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="W107" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="X107" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC107" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD107" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE107" s="7"/>
+      <c r="AF107" s="7"/>
+      <c r="AG107" s="7"/>
+      <c r="AH107" s="7"/>
+      <c r="AI107" s="7"/>
+      <c r="AJ107" s="7"/>
+      <c r="AK107" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:37">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2025103379</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F108" s="3">
+        <v>4154</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="N108" s="3">
+        <v>5803</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T108" s="3">
+        <v>1</v>
+      </c>
+      <c r="U108" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="Y108" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="Z108" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC108" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="AD108" s="3"/>
+      <c r="AE108" s="3"/>
+      <c r="AF108" s="3"/>
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:37">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="7">
+        <v>2025103380</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F109" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N109" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="P109" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="Q109" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T109" s="7">
+        <v>1</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V109" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="W109" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="X109" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="Y109" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="Z109" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC109" s="9" t="s">
+        <v>755</v>
+      </c>
+      <c r="AD109" s="7"/>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
+      <c r="AG109" s="7"/>
+      <c r="AH109" s="7"/>
+      <c r="AI109" s="7"/>
+      <c r="AJ109" s="7"/>
+      <c r="AK109" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2025103385</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="Y110" s="3"/>
+      <c r="Z110" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC110" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD110" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:37">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C111" s="7">
+        <v>2025103386</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7">
+        <v>2303</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T111" s="7">
+        <v>1</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V111" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="W111" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="Y111" s="7"/>
+      <c r="Z111" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC111" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD111" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="7"/>
+      <c r="AH111" s="7"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="7"/>
+      <c r="AK111" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:37">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2025103387</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3">
+        <v>2935</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S112" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T112" s="3">
+        <v>1</v>
+      </c>
+      <c r="U112" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="X112" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="Y112" s="3"/>
+      <c r="Z112" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC112" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD112" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE112" s="3"/>
+      <c r="AF112" s="3"/>
+      <c r="AG112" s="3"/>
+      <c r="AH112" s="3"/>
+      <c r="AI112" s="3"/>
+      <c r="AJ112" s="3"/>
+      <c r="AK112" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:37">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C113" s="7">
+        <v>2025103398</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7">
+        <v>4154</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="7"/>
+      <c r="O113" s="8"/>
+      <c r="P113" s="9"/>
+      <c r="Q113" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="R113" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T113" s="7">
+        <v>1</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V113" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="W113" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="X113" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="Y113" s="7"/>
+      <c r="Z113" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC113" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD113" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE113" s="7"/>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="7"/>
+      <c r="AH113" s="7"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK113" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="114" spans="1:37">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2025103409</v>
+      </c>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T114" s="3">
+        <v>1</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="Y114" s="3"/>
+      <c r="Z114" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC114" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="AD114" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE114" s="3"/>
+      <c r="AF114" s="3"/>
+      <c r="AG114" s="3"/>
+      <c r="AH114" s="3"/>
+      <c r="AI114" s="3"/>
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10291315
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$114</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$119</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="767">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-28  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="793">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-29  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2222,6 +2222,36 @@
     <t>2025-10-28 12:20:00</t>
   </si>
   <si>
+    <t>13380114102801</t>
+  </si>
+  <si>
+    <t>北縣莊勝店</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:40:47</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)游標亂跳並發出逼聲，與門市確認螢幕無任何文宣與商品放置並已重新開關機仍異常，因亂跳嚴重無法觸控校正...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03380</t>
+  </si>
+  <si>
+    <t>2025-10-28 12:45:10</t>
+  </si>
+  <si>
+    <t>2025-10-29 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 16:45:00</t>
+  </si>
+  <si>
+    <t>重插排線 清潔螢幕 觸控校正</t>
+  </si>
+  <si>
     <t>三重大院店</t>
   </si>
   <si>
@@ -2340,6 +2370,39 @@
     <t>供電異常導致主機開機error&amp;螢幕顯示異常，經放電後測試功能正常，請門市觀察中</t>
   </si>
   <si>
+    <t>E3601114102801</t>
+  </si>
+  <si>
+    <t>三重重富店</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:22:34</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD)會不定時變成藍屏，很傷眼睛，門市已重新拔插後方線路仍異常....須請台芝到店協助(螢幕變藍很傷眼睛)
+10/28  15:28  請門市先拔插線路， 稍晚再去電確認...廖</t>
+  </si>
+  <si>
+    <t>THILF03601</t>
+  </si>
+  <si>
+    <t>2025-10-28 15:46:21</t>
+  </si>
+  <si>
+    <t>2025-10-29 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-29 19:46:00</t>
+  </si>
+  <si>
+    <t>更換螢幕
+換上8133003791
+換下8133002586</t>
+  </si>
+  <si>
     <t>2025-10-28 15:48:53</t>
   </si>
   <si>
@@ -2371,6 +2434,24 @@
   </si>
   <si>
     <t>PMQ4+L99</t>
+  </si>
+  <si>
+    <t>2025-10-28 18:47:43</t>
+  </si>
+  <si>
+    <t>2025-10-28 18:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 18:45:00</t>
+  </si>
+  <si>
+    <t>2025-10-28 18:56:52</t>
+  </si>
+  <si>
+    <t>2025-10-29 10:56:10</t>
+  </si>
+  <si>
+    <t>2025-10-29 09:30:00</t>
   </si>
 </sst>
 </file>
@@ -2784,10 +2865,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK114"/>
+  <dimension ref="A1:AK119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC111" sqref="AC111"/>
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11567,38 +11648,58 @@
         <v>102</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C104" s="3">
-        <v>2025103352</v>
-      </c>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
+        <v>2025103351</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F104" s="3">
-        <v>4560</v>
+        <v>3380</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N104" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O104" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>720</v>
+      </c>
       <c r="Q104" s="3" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="R104" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S104" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="T104" s="3">
         <v>1</v>
@@ -11607,28 +11708,28 @@
         <v>54</v>
       </c>
       <c r="V104" s="3" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="W104" s="3" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="X104" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="Y104" s="3"/>
+        <v>724</v>
+      </c>
+      <c r="Y104" s="3" t="s">
+        <v>725</v>
+      </c>
       <c r="Z104" s="3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AA104" s="3"/>
       <c r="AB104" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC104" s="10" t="s">
-        <v>697</v>
-      </c>
-      <c r="AD104" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>726</v>
+      </c>
+      <c r="AD104" s="3"/>
       <c r="AE104" s="3"/>
       <c r="AF104" s="3"/>
       <c r="AG104" s="3"/>
@@ -11647,15 +11748,15 @@
         <v>92</v>
       </c>
       <c r="C105" s="7">
-        <v>2025103356</v>
+        <v>2025103352</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7">
-        <v>2935</v>
+        <v>4560</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c r="H105" s="7" t="s">
         <v>98</v>
@@ -11669,7 +11770,7 @@
       <c r="O105" s="8"/>
       <c r="P105" s="9"/>
       <c r="Q105" s="7" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="R105" s="7" t="s">
         <v>52</v>
@@ -11684,17 +11785,17 @@
         <v>54</v>
       </c>
       <c r="V105" s="7" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="W105" s="7" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="X105" s="7" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="Y105" s="7"/>
       <c r="Z105" s="7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA105" s="7"/>
       <c r="AB105" s="7" t="s">
@@ -11724,18 +11825,18 @@
         <v>92</v>
       </c>
       <c r="C106" s="3">
-        <v>2025103369</v>
+        <v>2025103356</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3">
-        <v>4715</v>
+        <v>2935</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>728</v>
+        <v>98</v>
       </c>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
@@ -11746,13 +11847,13 @@
       <c r="O106" s="4"/>
       <c r="P106" s="10"/>
       <c r="Q106" s="3" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="R106" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S106" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="T106" s="3">
         <v>1</v>
@@ -11761,13 +11862,13 @@
         <v>54</v>
       </c>
       <c r="V106" s="3" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="W106" s="3" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="X106" s="3" t="s">
-        <v>687</v>
+        <v>736</v>
       </c>
       <c r="Y106" s="3"/>
       <c r="Z106" s="3">
@@ -11788,9 +11889,7 @@
       <c r="AG106" s="3"/>
       <c r="AH106" s="3"/>
       <c r="AI106" s="3"/>
-      <c r="AJ106" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ106" s="3"/>
       <c r="AK106" s="3" t="s">
         <v>61</v>
       </c>
@@ -11803,18 +11902,18 @@
         <v>92</v>
       </c>
       <c r="C107" s="7">
-        <v>2025103375</v>
+        <v>2025103369</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7">
-        <v>2042</v>
+        <v>4715</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>98</v>
+        <v>738</v>
       </c>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
@@ -11825,13 +11924,13 @@
       <c r="O107" s="8"/>
       <c r="P107" s="9"/>
       <c r="Q107" s="7" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="R107" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S107" s="7" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="T107" s="7">
         <v>1</v>
@@ -11840,17 +11939,17 @@
         <v>54</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="W107" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="X107" s="7" t="s">
         <v>687</v>
-      </c>
-      <c r="X107" s="7" t="s">
-        <v>735</v>
       </c>
       <c r="Y107" s="7"/>
       <c r="Z107" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA107" s="7"/>
       <c r="AB107" s="7" t="s">
@@ -11867,7 +11966,9 @@
       <c r="AG107" s="7"/>
       <c r="AH107" s="7"/>
       <c r="AI107" s="7"/>
-      <c r="AJ107" s="7"/>
+      <c r="AJ107" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AK107" s="7" t="s">
         <v>61</v>
       </c>
@@ -11877,58 +11978,38 @@
         <v>106</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="C108" s="3">
-        <v>2025103379</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>2025103375</v>
+      </c>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
       <c r="F108" s="3">
-        <v>4154</v>
+        <v>2042</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>738</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K108" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L108" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="M108" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="N108" s="3">
-        <v>5803</v>
-      </c>
-      <c r="O108" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="P108" s="10" t="s">
-        <v>739</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="10"/>
       <c r="Q108" s="3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="R108" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="T108" s="3">
         <v>1</v>
@@ -11937,28 +12018,28 @@
         <v>54</v>
       </c>
       <c r="V108" s="3" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="W108" s="3" t="s">
-        <v>742</v>
+        <v>687</v>
       </c>
       <c r="X108" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="Y108" s="3" t="s">
-        <v>744</v>
-      </c>
+        <v>745</v>
+      </c>
+      <c r="Y108" s="3"/>
       <c r="Z108" s="3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AA108" s="3"/>
       <c r="AB108" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC108" s="10" t="s">
-        <v>745</v>
-      </c>
-      <c r="AD108" s="3"/>
+        <v>697</v>
+      </c>
+      <c r="AD108" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="AE108" s="3"/>
       <c r="AF108" s="3"/>
       <c r="AG108" s="3"/>
@@ -11977,7 +12058,7 @@
         <v>38</v>
       </c>
       <c r="C109" s="7">
-        <v>2025103380</v>
+        <v>2025103379</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>746</v>
@@ -11986,13 +12067,13 @@
         <v>40</v>
       </c>
       <c r="F109" s="7">
-        <v>5364</v>
+        <v>4154</v>
       </c>
       <c r="G109" s="7" t="s">
         <v>747</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>728</v>
+        <v>738</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>748</v>
@@ -12004,16 +12085,16 @@
         <v>100</v>
       </c>
       <c r="L109" s="7" t="s">
-        <v>115</v>
+        <v>571</v>
       </c>
       <c r="M109" s="8" t="s">
-        <v>116</v>
+        <v>572</v>
       </c>
       <c r="N109" s="7">
-        <v>2306</v>
+        <v>5803</v>
       </c>
       <c r="O109" s="8" t="s">
-        <v>117</v>
+        <v>494</v>
       </c>
       <c r="P109" s="9" t="s">
         <v>749</v>
@@ -12046,7 +12127,7 @@
         <v>754</v>
       </c>
       <c r="Z109" s="7">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="AA109" s="7"/>
       <c r="AB109" s="7" t="s">
@@ -12071,38 +12152,58 @@
         <v>108</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C110" s="3">
-        <v>2025103385</v>
-      </c>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3" t="s">
-        <v>680</v>
+        <v>2025103380</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F110" s="3">
+        <v>5364</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>681</v>
+        <v>757</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="3"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="10"/>
+        <v>738</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N110" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>759</v>
+      </c>
       <c r="Q110" s="3" t="s">
-        <v>685</v>
+        <v>760</v>
       </c>
       <c r="R110" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="T110" s="3">
         <v>1</v>
@@ -12111,28 +12212,28 @@
         <v>54</v>
       </c>
       <c r="V110" s="3" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>687</v>
+        <v>762</v>
       </c>
       <c r="X110" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="Y110" s="3"/>
+        <v>763</v>
+      </c>
+      <c r="Y110" s="3" t="s">
+        <v>764</v>
+      </c>
       <c r="Z110" s="3">
-        <v>0.8</v>
+        <v>1.7</v>
       </c>
       <c r="AA110" s="3"/>
       <c r="AB110" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC110" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD110" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>765</v>
+      </c>
+      <c r="AD110" s="3"/>
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
@@ -12148,38 +12249,58 @@
         <v>109</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C111" s="7">
-        <v>2025103386</v>
-      </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
+        <v>2025103384</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F111" s="7">
-        <v>2303</v>
+        <v>3601</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I111" s="7"/>
-      <c r="J111" s="7"/>
-      <c r="K111" s="7"/>
-      <c r="L111" s="7"/>
-      <c r="M111" s="8"/>
-      <c r="N111" s="7"/>
-      <c r="O111" s="8"/>
-      <c r="P111" s="9"/>
+      <c r="I111" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="N111" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="P111" s="9" t="s">
+        <v>769</v>
+      </c>
       <c r="Q111" s="7" t="s">
-        <v>759</v>
+        <v>770</v>
       </c>
       <c r="R111" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S111" s="7" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="T111" s="7">
         <v>1</v>
@@ -12188,28 +12309,28 @@
         <v>54</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>760</v>
+        <v>771</v>
       </c>
       <c r="W111" s="7" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="X111" s="7" t="s">
-        <v>761</v>
-      </c>
-      <c r="Y111" s="7"/>
+        <v>773</v>
+      </c>
+      <c r="Y111" s="7" t="s">
+        <v>774</v>
+      </c>
       <c r="Z111" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA111" s="7"/>
       <c r="AB111" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC111" s="9" t="s">
-        <v>697</v>
-      </c>
-      <c r="AD111" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>775</v>
+      </c>
+      <c r="AD111" s="7"/>
       <c r="AE111" s="7"/>
       <c r="AF111" s="7"/>
       <c r="AG111" s="7"/>
@@ -12228,18 +12349,18 @@
         <v>92</v>
       </c>
       <c r="C112" s="3">
-        <v>2025103387</v>
+        <v>2025103385</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="3">
-        <v>2935</v>
+      <c r="F112" s="3" t="s">
+        <v>680</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>722</v>
+        <v>681</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
@@ -12250,13 +12371,13 @@
       <c r="O112" s="4"/>
       <c r="P112" s="10"/>
       <c r="Q112" s="3" t="s">
-        <v>723</v>
+        <v>685</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="T112" s="3">
         <v>1</v>
@@ -12265,24 +12386,24 @@
         <v>54</v>
       </c>
       <c r="V112" s="3" t="s">
-        <v>762</v>
+        <v>776</v>
       </c>
       <c r="W112" s="3" t="s">
-        <v>742</v>
+        <v>687</v>
       </c>
       <c r="X112" s="3" t="s">
-        <v>763</v>
+        <v>777</v>
       </c>
       <c r="Y112" s="3"/>
       <c r="Z112" s="3">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="AA112" s="3"/>
       <c r="AB112" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC112" s="10" t="s">
-        <v>697</v>
+        <v>95</v>
       </c>
       <c r="AD112" s="3" t="s">
         <v>61</v>
@@ -12305,18 +12426,18 @@
         <v>92</v>
       </c>
       <c r="C113" s="7">
-        <v>2025103398</v>
+        <v>2025103386</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7">
-        <v>4154</v>
+        <v>2303</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>737</v>
+        <v>778</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>728</v>
+        <v>98</v>
       </c>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
@@ -12327,13 +12448,13 @@
       <c r="O113" s="8"/>
       <c r="P113" s="9"/>
       <c r="Q113" s="7" t="s">
-        <v>740</v>
+        <v>779</v>
       </c>
       <c r="R113" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S113" s="7" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="T113" s="7">
         <v>1</v>
@@ -12342,17 +12463,17 @@
         <v>54</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>764</v>
+        <v>780</v>
       </c>
       <c r="W113" s="7" t="s">
-        <v>687</v>
+        <v>735</v>
       </c>
       <c r="X113" s="7" t="s">
-        <v>742</v>
+        <v>781</v>
       </c>
       <c r="Y113" s="7"/>
       <c r="Z113" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA113" s="7"/>
       <c r="AB113" s="7" t="s">
@@ -12369,9 +12490,7 @@
       <c r="AG113" s="7"/>
       <c r="AH113" s="7"/>
       <c r="AI113" s="7"/>
-      <c r="AJ113" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ113" s="7"/>
       <c r="AK113" s="7" t="s">
         <v>61</v>
       </c>
@@ -12384,18 +12503,18 @@
         <v>92</v>
       </c>
       <c r="C114" s="3">
-        <v>2025103409</v>
+        <v>2025103387</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="3" t="s">
-        <v>680</v>
+      <c r="F114" s="3">
+        <v>2935</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>681</v>
+        <v>732</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
@@ -12404,15 +12523,15 @@
       <c r="M114" s="4"/>
       <c r="N114" s="3"/>
       <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
+      <c r="P114" s="10"/>
       <c r="Q114" s="3" t="s">
-        <v>685</v>
+        <v>733</v>
       </c>
       <c r="R114" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="T114" s="3">
         <v>1</v>
@@ -12421,24 +12540,24 @@
         <v>54</v>
       </c>
       <c r="V114" s="3" t="s">
-        <v>765</v>
+        <v>782</v>
       </c>
       <c r="W114" s="3" t="s">
-        <v>687</v>
+        <v>752</v>
       </c>
       <c r="X114" s="3" t="s">
-        <v>688</v>
+        <v>783</v>
       </c>
       <c r="Y114" s="3"/>
       <c r="Z114" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="AA114" s="3"/>
       <c r="AB114" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC114" s="4" t="s">
-        <v>766</v>
+      <c r="AC114" s="10" t="s">
+        <v>697</v>
       </c>
       <c r="AD114" s="3" t="s">
         <v>61</v>
@@ -12450,6 +12569,397 @@
       <c r="AI114" s="3"/>
       <c r="AJ114" s="3"/>
       <c r="AK114" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2025103398</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7">
+        <v>4154</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK115" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2025103409</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3"/>
+      <c r="AK116" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2025103411</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD117" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK117" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2025103412</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD118" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3"/>
+      <c r="AK118" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2025103439</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7">
+        <v>3380</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="8"/>
+      <c r="Q119" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC119" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD119" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK119" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10301718
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$119</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$122</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="793">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-29  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="810">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-30  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2452,6 +2452,57 @@
   </si>
   <si>
     <t>2025-10-29 09:30:00</t>
+  </si>
+  <si>
+    <t>板橋藝文中心</t>
+  </si>
+  <si>
+    <t>THILF03399</t>
+  </si>
+  <si>
+    <t>2025-10-30 10:58:58</t>
+  </si>
+  <si>
+    <t>2025-10-30 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-30 11:00:00</t>
+  </si>
+  <si>
+    <t>撤店</t>
+  </si>
+  <si>
+    <t>三重鑫五華</t>
+  </si>
+  <si>
+    <t>THILF05457</t>
+  </si>
+  <si>
+    <t>2025-10-30 15:00:05</t>
+  </si>
+  <si>
+    <t>2025-10-30 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-30 15:00:00</t>
+  </si>
+  <si>
+    <t>新開門市</t>
+  </si>
+  <si>
+    <t>三重中央南</t>
+  </si>
+  <si>
+    <t>THILF04083</t>
+  </si>
+  <si>
+    <t>2025-10-30 16:04:12</t>
+  </si>
+  <si>
+    <t>2025-10-30 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-30 16:00:00</t>
   </si>
 </sst>
 </file>
@@ -2865,10 +2916,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK119"/>
+  <dimension ref="A1:AK122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="AC119" sqref="AC119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12912,7 +12963,7 @@
       <c r="M119" s="8"/>
       <c r="N119" s="7"/>
       <c r="O119" s="8"/>
-      <c r="P119" s="8"/>
+      <c r="P119" s="9"/>
       <c r="Q119" s="7" t="s">
         <v>721</v>
       </c>
@@ -12945,7 +12996,7 @@
       <c r="AB119" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC119" s="8" t="s">
+      <c r="AC119" s="9" t="s">
         <v>697</v>
       </c>
       <c r="AD119" s="7" t="s">
@@ -12960,6 +13011,237 @@
         <v>61</v>
       </c>
       <c r="AK119" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2025103523</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>3399</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="AD120" s="3"/>
+      <c r="AE120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3"/>
+      <c r="AK120" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2025103585</v>
+      </c>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7">
+        <v>5457</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="9"/>
+      <c r="Q121" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC121" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="AD121" s="7"/>
+      <c r="AE121" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2025103613</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>4083</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC122" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="AD122" s="3"/>
+      <c r="AE122" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3"/>
+      <c r="AK122" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10311245
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$122</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$126</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="810">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-30  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="838">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-31  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2454,6 +2454,30 @@
     <t>2025-10-29 09:30:00</t>
   </si>
   <si>
+    <t>14144114103002</t>
+  </si>
+  <si>
+    <t>2025-10-30 10:21:50</t>
+  </si>
+  <si>
+    <t>門市門市反應印票機L90 paper燈號亮紅燈，已有關機紙捲重裝列印測試票券仍亮紅燈無法出票....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-10-30 10:24:04</t>
+  </si>
+  <si>
+    <t>2025-10-31 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 14:24:00</t>
+  </si>
+  <si>
+    <t>重插電源 更新韌體</t>
+  </si>
+  <si>
     <t>板橋藝文中心</t>
   </si>
   <si>
@@ -2503,6 +2527,67 @@
   </si>
   <si>
     <t>2025-10-30 16:00:00</t>
+  </si>
+  <si>
+    <t>E4282114103001</t>
+  </si>
+  <si>
+    <t>林口建林店</t>
+  </si>
+  <si>
+    <t>2025-10-30 17:39:28</t>
+  </si>
+  <si>
+    <t>門市反應 MMK 四代機 熱感機T70II列印小白單無反應，燈號為綠燈，已有重啟熱感機+MMK仍異常...請台芝到店協助	(無法出紙)</t>
+  </si>
+  <si>
+    <t>THILF04282</t>
+  </si>
+  <si>
+    <t>2025-10-30 17:49:28</t>
+  </si>
+  <si>
+    <t>2025-10-31 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 21:49:00</t>
+  </si>
+  <si>
+    <t>客戶取消 現場為L90故障</t>
+  </si>
+  <si>
+    <t>E3380114103101</t>
+  </si>
+  <si>
+    <t>2025-10-31 02:08:26</t>
+  </si>
+  <si>
+    <t>當機</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)這兩天常發生使用到一半會突然黑屏關機，隔很久TM自動自行重啟，門市已有檢察後方變壓器、插頭都有插緊未鬆脫，希望工程師到店檢察....須請台芝到店協助(沒反應無法開機)
+10/31 09:02  請門市繁忙，稍晚聯繫...廖</t>
+  </si>
+  <si>
+    <t>2025-10-31 09:25:59</t>
+  </si>
+  <si>
+    <t>2025-10-31 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-11-03 13:26:00</t>
+  </si>
+  <si>
+    <t>變壓器端接觸不良，重新固定排線</t>
+  </si>
+  <si>
+    <t>2025-10-31 10:40:29</t>
+  </si>
+  <si>
+    <t>2025-10-31 09:00:00</t>
   </si>
 </sst>
 </file>
@@ -2916,10 +3001,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK122"/>
+  <dimension ref="A1:AK126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC119" sqref="AC119"/>
+      <selection activeCell="AC123" sqref="AC123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13019,32 +13104,52 @@
         <v>118</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C120" s="3">
-        <v>2025103523</v>
-      </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
+        <v>2025103520</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F120" s="3">
-        <v>3399</v>
+        <v>4144</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>793</v>
+        <v>658</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="3"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="10"/>
+        <v>81</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K120" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="M120" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="N120" s="3">
+        <v>6003</v>
+      </c>
+      <c r="O120" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P120" s="10" t="s">
+        <v>795</v>
+      </c>
       <c r="Q120" s="3" t="s">
-        <v>794</v>
+        <v>662</v>
       </c>
       <c r="R120" s="3" t="s">
         <v>52</v>
@@ -13059,15 +13164,17 @@
         <v>54</v>
       </c>
       <c r="V120" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="W120" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="X120" s="3" t="s">
-        <v>797</v>
-      </c>
-      <c r="Y120" s="3"/>
+        <v>798</v>
+      </c>
+      <c r="Y120" s="3" t="s">
+        <v>799</v>
+      </c>
       <c r="Z120" s="3">
         <v>0.5</v>
       </c>
@@ -13076,12 +13183,10 @@
         <v>59</v>
       </c>
       <c r="AC120" s="10" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="AD120" s="3"/>
-      <c r="AE120" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE120" s="3"/>
       <c r="AF120" s="3"/>
       <c r="AG120" s="3"/>
       <c r="AH120" s="3"/>
@@ -13099,18 +13204,18 @@
         <v>92</v>
       </c>
       <c r="C121" s="7">
-        <v>2025103585</v>
+        <v>2025103523</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7">
-        <v>5457</v>
+        <v>3399</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
@@ -13121,7 +13226,7 @@
       <c r="O121" s="8"/>
       <c r="P121" s="9"/>
       <c r="Q121" s="7" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="R121" s="7" t="s">
         <v>52</v>
@@ -13136,24 +13241,24 @@
         <v>54</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="W121" s="7" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="X121" s="7" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="Y121" s="7"/>
       <c r="Z121" s="7">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AA121" s="7"/>
       <c r="AB121" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC121" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="AD121" s="7"/>
       <c r="AE121" s="7" t="s">
@@ -13176,15 +13281,15 @@
         <v>92</v>
       </c>
       <c r="C122" s="3">
-        <v>2025103613</v>
+        <v>2025103585</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3">
-        <v>4083</v>
+        <v>5457</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>98</v>
@@ -13196,9 +13301,9 @@
       <c r="M122" s="4"/>
       <c r="N122" s="3"/>
       <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
+      <c r="P122" s="10"/>
       <c r="Q122" s="3" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="R122" s="3" t="s">
         <v>52</v>
@@ -13213,24 +13318,24 @@
         <v>54</v>
       </c>
       <c r="V122" s="3" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="W122" s="3" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="X122" s="3" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="Y122" s="3"/>
       <c r="Z122" s="3">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="AA122" s="3"/>
       <c r="AB122" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC122" s="4" t="s">
-        <v>798</v>
+      <c r="AC122" s="10" t="s">
+        <v>812</v>
       </c>
       <c r="AD122" s="3"/>
       <c r="AE122" s="3" t="s">
@@ -13242,6 +13347,356 @@
       <c r="AI122" s="3"/>
       <c r="AJ122" s="3"/>
       <c r="AK122" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2025103613</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7">
+        <v>4083</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2025103647</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F124" s="3">
+        <v>4282</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L124" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M124" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N124" s="3">
+        <v>5903</v>
+      </c>
+      <c r="O124" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P124" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q124" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="Y124" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="Z124" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>827</v>
+      </c>
+      <c r="AD124" s="3"/>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2025103655</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="7">
+        <v>3380</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N125" s="7">
+        <v>2301</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="P125" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q125" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="Y125" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="Z125" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="AD125" s="7"/>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2025103669</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <v>4282</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y126" s="3"/>
+      <c r="Z126" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC126" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD126" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK126" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 10311754
</commit_message>
<xml_diff>
--- a/IM/202510_HL_Maintain_Report.xlsx
+++ b/IM/202510_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$126</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$128</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="847">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202510   (  製表日期:2025-10-31  )</t>
   </si>
@@ -2588,6 +2588,33 @@
   </si>
   <si>
     <t>2025-10-31 09:00:00</t>
+  </si>
+  <si>
+    <t>新莊化成店</t>
+  </si>
+  <si>
+    <t>THILF02362</t>
+  </si>
+  <si>
+    <t>2025-10-31 13:11:06</t>
+  </si>
+  <si>
+    <t>2025-10-31 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 13:20:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 14:30:58</t>
+  </si>
+  <si>
+    <t>2025-10-31 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-10-31 14:30:00</t>
+  </si>
+  <si>
+    <t>PEP裝機完成</t>
   </si>
 </sst>
 </file>
@@ -3001,10 +3028,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK126"/>
+  <dimension ref="A1:AK128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC123" sqref="AC123"/>
+      <selection activeCell="AC125" sqref="AC125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13649,7 +13676,7 @@
       <c r="M126" s="4"/>
       <c r="N126" s="3"/>
       <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
+      <c r="P126" s="10"/>
       <c r="Q126" s="3" t="s">
         <v>822</v>
       </c>
@@ -13682,7 +13709,7 @@
       <c r="AB126" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC126" s="4" t="s">
+      <c r="AC126" s="10" t="s">
         <v>697</v>
       </c>
       <c r="AD126" s="3" t="s">
@@ -13697,6 +13724,162 @@
         <v>61</v>
       </c>
       <c r="AK126" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2025103693</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>2362</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK127" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2025103704</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <v>5457</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y128" s="3"/>
+      <c r="Z128" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC128" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="AD128" s="3"/>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK128" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>